<commit_message>
Add allowed values validation
</commit_message>
<xml_diff>
--- a/table1.xlsx
+++ b/table1.xlsx
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1086,7 +1086,7 @@
         <v>20</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>3</v>

</xml_diff>

<commit_message>
Add json output & fix bugs
</commit_message>
<xml_diff>
--- a/table1.xlsx
+++ b/table1.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21780" windowHeight="10335" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21780" windowHeight="10335" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="_comment" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet_1_1" sheetId="3" r:id="rId1"/>
+    <sheet name="sheet_1_2" sheetId="4" r:id="rId2"/>
+    <sheet name="_comment" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>any thing here</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -108,13 +109,6 @@
     "dataType" : "string",
     "minLen" : 3,
     "maxLen" : 30
-}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-    "dataType" : "ref",
-    "ref" : "table2:sheet1"
 }</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -191,6 +185,13 @@
     "minLen" : 3,
     "maxLen" : 30,
     "regExp" : "[1-9]*"
+}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "dataType" : "ref",
+    "ref" : "table2:sheet_2_1"
 }</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -566,10 +567,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1015,7 +1016,7 @@
     </row>
     <row r="4" spans="1:8" s="9" customFormat="1" ht="171">
       <c r="A4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
@@ -1033,10 +1034,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1047,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1073,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1099,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1108,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="4">
         <v>123</v>
@@ -1125,6 +1126,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="2" width="27.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="9" customFormat="1" ht="71.25">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -1163,16 +1223,16 @@
       <c r="J2" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>